<commit_message>
Modul Informasi : Memperbaiki tampilan edit slip gaji
</commit_message>
<xml_diff>
--- a/tests/Form Import No Rekening.xlsx
+++ b/tests/Form Import No Rekening.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="22">
   <si>
     <t>Nama Bank</t>
   </si>
@@ -148,7 +148,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -158,6 +158,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -439,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,7 +478,7 @@
       <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -492,7 +495,7 @@
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -509,7 +512,7 @@
       <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -526,7 +529,7 @@
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -534,6 +537,74 @@
       </c>
       <c r="E5" s="2" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="4">
+        <v>982374982374</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="4">
+        <v>6723942389</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="4">
+        <v>932402093</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="4">
+        <v>8792347234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>